<commit_message>
more things more results
</commit_message>
<xml_diff>
--- a/March 2023/Waypoints Model/results.xlsx
+++ b/March 2023/Waypoints Model/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sixtium\Documents\GitStuff\AWSDeepracer\March 2023\Waypoints Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ADA2AE-2B3A-4194-850F-6521BC6BC1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD72DC7-39C2-4156-9D04-CEDD23C01961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
   <si>
     <t>Model Name</t>
   </si>
@@ -148,6 +148,123 @@
   </si>
   <si>
     <t>WaypointModel-RacingLineWeightIs6-ClockWise-50min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs6-ClockWise-60min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs7-ClockWise-70min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs5-ClockWise-80min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs5-ClockWise-90min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs8-ClockWise-120min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs8-ClockWise-150min-clone-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs8-ClockWise-180min-clone-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs5-ClockWise-240min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs6-ClockWise-270min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs9-ClockWise-300min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs9-ClockWise-330min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs7-ClockWise-400min-clone</t>
+  </si>
+  <si>
+    <t>research_model_v2</t>
+  </si>
+  <si>
+    <t>FastAroundTrackSquared-3h</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs7-ClockWise-430min-clone</t>
+  </si>
+  <si>
+    <t>AlexHamilton</t>
+  </si>
+  <si>
+    <t>FastAroundTrackSquared-5h-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs7-ClockWise-500min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs8-ClockWise-530min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs8-ClockWise-600min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs7-ClockWise-630min-clone</t>
+  </si>
+  <si>
+    <t>FastAroundTrackSquared-7h-clone-clone</t>
+  </si>
+  <si>
+    <t>FastAroundTrackSquared-10h-clone-clone-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs9-ClockWise-700min-clone</t>
+  </si>
+  <si>
+    <t>WaypointModel-RacingLineWeightIs4-ClockWise-730min-clone</t>
+  </si>
+  <si>
+    <t>research_model_v3</t>
+  </si>
+  <si>
+    <t>YourLocalPasonite</t>
+  </si>
+  <si>
+    <t>myrewardfunction3-3h</t>
+  </si>
+  <si>
+    <t>myrewardfunction3-6h-clone</t>
+  </si>
+  <si>
+    <t>research_model_v4</t>
+  </si>
+  <si>
+    <t>myrewardfunction3-8h-clone-clone</t>
+  </si>
+  <si>
+    <t>NotChatGPT3</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>research_model_v5</t>
+  </si>
+  <si>
+    <t>myrewardfunction3-9h-clone-clone</t>
+  </si>
+  <si>
+    <t>research_model_v6</t>
+  </si>
+  <si>
+    <t>myrewardfunction6-10h-clone-clone-clone</t>
   </si>
 </sst>
 </file>
@@ -189,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -219,6 +336,7 @@
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +591,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$25:$D$33</c:f>
+              <c:f>Sheet1!$D$25:$D$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -491,16 +609,82 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>730</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$25:$K$33</c:f>
+              <c:f>Sheet1!$K$25:$K$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>571.46100000000001</c:v>
                 </c:pt>
@@ -515,6 +699,72 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>356.32299999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>356.32299999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>353.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>353.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>353.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>353.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>281.94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>250.012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>250.012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>250.012</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>250.012</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>250.012</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>243.124</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>243.124</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>220.524</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>220.524</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>220.524</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220.524</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>215.99100000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>215.99100000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>215.99100000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>215.99100000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>215.99100000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -523,6 +773,178 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-4753-4FF3-A93B-B70DDF7FA14D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AlexHamilton</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$54:$D$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$54:$K$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>237.12799999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230.19300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230.19300000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230.19300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4753-4FF3-A93B-B70DDF7FA14D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>YourLocalPasonite</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$59:$D$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$59:$K$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>230.13800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227.922</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>221.66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>221.45599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>221.45599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4753-4FF3-A93B-B70DDF7FA14D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -603,6 +1025,8 @@
         <c:axId val="809691695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="300"/>
+          <c:min val="200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1305,15 +1729,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>122872</xdr:rowOff>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>92392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>149542</xdr:rowOff>
+      <xdr:colOff>283845</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1604,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="K15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1799,7 +2223,7 @@
         <v>7</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F29" si="2">10-E7</f>
+        <f t="shared" ref="F7:F32" si="2">10-E7</f>
         <v>3</v>
       </c>
       <c r="G7">
@@ -2500,221 +2924,1557 @@
       <c r="A25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="5">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="5">
         <v>10</v>
       </c>
-      <c r="E25" s="9" t="str">
+      <c r="E25" s="6" t="str">
         <f>RIGHT(LEFT(C25,33),1)</f>
         <v>5</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="5">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="5">
         <v>9</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="5">
         <v>31</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="5">
         <v>461</v>
       </c>
-      <c r="J25" s="10" t="str">
+      <c r="J25" s="5" t="str">
         <f t="shared" si="23"/>
         <v>9:31.461</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="5">
         <f t="shared" si="24"/>
         <v>571.46100000000001</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="13">
         <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
-      <c r="B26">
+      <c r="B26" s="5">
         <v>2</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="5">
         <v>20</v>
       </c>
-      <c r="E26" s="9" t="str">
+      <c r="E26" s="6" t="str">
         <f>RIGHT(LEFT(C26,33),1)</f>
         <v>6</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="5">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="5">
         <v>8</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="5">
         <v>24</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="5">
         <v>145</v>
       </c>
-      <c r="J26" s="10" t="str">
+      <c r="J26" s="5" t="str">
         <f t="shared" si="23"/>
         <v>8:24.145</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="5">
         <f t="shared" si="24"/>
         <v>504.14499999999998</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="13">
         <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
-      <c r="B27">
+      <c r="B27" s="5">
         <v>3</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="5">
         <v>30</v>
       </c>
-      <c r="E27" s="9" t="str">
+      <c r="E27" s="6" t="str">
         <f>RIGHT(LEFT(C27,33),1)</f>
         <v>6</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="5">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="5">
         <v>6</v>
       </c>
-      <c r="H27" t="str">
+      <c r="H27" s="5" t="str">
         <f>"01"</f>
         <v>01</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="5">
         <v>138</v>
       </c>
-      <c r="J27" s="10" t="str">
+      <c r="J27" s="5" t="str">
         <f t="shared" ref="J27" si="25">_xlfn.TEXTJOIN("",FALSE,G27,":",H27,".",I27)</f>
         <v>6:01.138</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K27" s="5">
         <f t="shared" ref="K27" si="26">(G27*60)+(H27)+(I27/1000)</f>
         <v>361.13799999999998</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="13">
         <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
-      <c r="B28">
+      <c r="B28" s="5">
         <v>4</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="5">
         <v>40</v>
       </c>
-      <c r="E28" s="9" t="str">
+      <c r="E28" s="6" t="str">
         <f>RIGHT(LEFT(C28,33),1)</f>
         <v>6</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="5">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="5">
         <v>5</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="5">
         <v>57</v>
       </c>
-      <c r="I28" t="str">
+      <c r="I28" s="5" t="str">
         <f>"130"</f>
         <v>130</v>
       </c>
-      <c r="J28" s="10" t="str">
+      <c r="J28" s="5" t="str">
         <f t="shared" ref="J28" si="27">_xlfn.TEXTJOIN("",FALSE,G28,":",H28,".",I28)</f>
         <v>5:57.130</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="5">
         <f t="shared" ref="K28" si="28">(G28*60)+(H28)+(I28/1000)</f>
         <v>357.13</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
-      <c r="B29">
+      <c r="B29" s="5">
         <v>5</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="5">
         <v>50</v>
       </c>
-      <c r="E29" s="9" t="str">
+      <c r="E29" s="6" t="str">
         <f>RIGHT(LEFT(C29,33),1)</f>
         <v>6</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="5">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="5">
         <v>5</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="5">
         <v>56</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="5">
         <v>323</v>
       </c>
-      <c r="J29" s="10" t="str">
+      <c r="J29" s="5" t="str">
         <f t="shared" ref="J29" si="29">_xlfn.TEXTJOIN("",FALSE,G29,":",H29,".",I29)</f>
         <v>5:56.323</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="5">
         <f t="shared" ref="K29" si="30">(G29*60)+(H29)+(I29/1000)</f>
         <v>356.32299999999998</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L29" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30">
+        <v>60</v>
+      </c>
+      <c r="E30" s="9" t="str">
+        <f>RIGHT(LEFT(C30,33),1)</f>
+        <v>6</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>56</v>
+      </c>
+      <c r="I30">
+        <v>323</v>
+      </c>
+      <c r="J30" s="10" t="str">
+        <f t="shared" ref="J30" si="31">_xlfn.TEXTJOIN("",FALSE,G30,":",H30,".",I30)</f>
+        <v>5:56.323</v>
+      </c>
+      <c r="K30" s="10">
+        <f t="shared" ref="K30" si="32">(G30*60)+(H30)+(I30/1000)</f>
+        <v>356.32299999999998</v>
+      </c>
+      <c r="L30" s="12">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
+      <c r="B31" s="5">
+        <v>7</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="5">
+        <v>70</v>
+      </c>
+      <c r="E31" s="6" t="str">
+        <f>RIGHT(LEFT(C31,33),1)</f>
+        <v>7</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G31" s="5">
+        <v>5</v>
+      </c>
+      <c r="H31" s="5">
+        <v>53</v>
+      </c>
+      <c r="I31" s="5" t="str">
+        <f>"990"</f>
+        <v>990</v>
+      </c>
+      <c r="J31" s="5" t="str">
+        <f t="shared" ref="J31" si="33">_xlfn.TEXTJOIN("",FALSE,G31,":",H31,".",I31)</f>
+        <v>5:53.990</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" ref="K31" si="34">(G31*60)+(H31)+(I31/1000)</f>
+        <v>353.99</v>
+      </c>
+      <c r="L31" s="13">
+        <v>39</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32">
+        <v>80</v>
+      </c>
+      <c r="E32" s="9" t="str">
+        <f>RIGHT(LEFT(C32,33),1)</f>
+        <v>5</v>
+      </c>
+      <c r="F32" s="10">
+        <f>10-E32</f>
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="H32">
+        <v>53</v>
+      </c>
+      <c r="I32" t="str">
+        <f>"990"</f>
+        <v>990</v>
+      </c>
+      <c r="J32" s="10" t="str">
+        <f t="shared" ref="J32" si="35">_xlfn.TEXTJOIN("",FALSE,G32,":",H32,".",I32)</f>
+        <v>5:53.990</v>
+      </c>
+      <c r="K32" s="10">
+        <f t="shared" ref="K32" si="36">(G32*60)+(H32)+(I32/1000)</f>
+        <v>353.99</v>
+      </c>
+      <c r="L32" s="12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33">
+        <v>80</v>
+      </c>
+      <c r="E33" s="9" t="str">
+        <f>RIGHT(LEFT(C33,33),1)</f>
+        <v>5</v>
+      </c>
+      <c r="F33" s="10">
+        <f>10-E33</f>
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33">
+        <v>53</v>
+      </c>
+      <c r="I33" t="str">
+        <f>"990"</f>
+        <v>990</v>
+      </c>
+      <c r="J33" s="10" t="str">
+        <f t="shared" ref="J33" si="37">_xlfn.TEXTJOIN("",FALSE,G33,":",H33,".",I33)</f>
+        <v>5:53.990</v>
+      </c>
+      <c r="K33" s="10">
+        <f t="shared" ref="K33" si="38">(G33*60)+(H33)+(I33/1000)</f>
+        <v>353.99</v>
+      </c>
+      <c r="L33" s="12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34">
+        <v>90</v>
+      </c>
+      <c r="E34" s="9" t="str">
+        <f>RIGHT(LEFT(C34,33),1)</f>
+        <v>5</v>
+      </c>
+      <c r="F34" s="10">
+        <f>10-E34</f>
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34">
+        <v>53</v>
+      </c>
+      <c r="I34" t="str">
+        <f>"990"</f>
+        <v>990</v>
+      </c>
+      <c r="J34" s="10" t="str">
+        <f t="shared" ref="J34:J36" si="39">_xlfn.TEXTJOIN("",FALSE,G34,":",H34,".",I34)</f>
+        <v>5:53.990</v>
+      </c>
+      <c r="K34" s="10">
+        <f t="shared" ref="K34:K36" si="40">(G34*60)+(H34)+(I34/1000)</f>
+        <v>353.99</v>
+      </c>
+      <c r="L34" s="12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="5">
+        <v>11</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="5">
+        <v>120</v>
+      </c>
+      <c r="E35" s="6" t="str">
+        <f>RIGHT(LEFT(C35,33),1)</f>
+        <v>8</v>
+      </c>
+      <c r="F35" s="5">
+        <f>10-E35</f>
+        <v>2</v>
+      </c>
+      <c r="G35" s="5">
+        <v>4</v>
+      </c>
+      <c r="H35" s="5">
+        <v>41</v>
+      </c>
+      <c r="I35" s="5" t="str">
+        <f>"940"</f>
+        <v>940</v>
+      </c>
+      <c r="J35" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>4:41.940</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" si="40"/>
+        <v>281.94</v>
+      </c>
+      <c r="L35" s="13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36">
+        <v>150</v>
+      </c>
+      <c r="E36" s="9" t="str">
+        <f>RIGHT(LEFT(C36,33),1)</f>
+        <v>8</v>
+      </c>
+      <c r="F36" s="10">
+        <f>10-E36</f>
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <v>10</v>
+      </c>
+      <c r="I36" t="str">
+        <f>"012"</f>
+        <v>012</v>
+      </c>
+      <c r="J36" s="10" t="str">
+        <f t="shared" si="39"/>
+        <v>4:10.012</v>
+      </c>
+      <c r="K36" s="10">
+        <f t="shared" si="40"/>
+        <v>250.012</v>
+      </c>
+      <c r="L36" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37">
+        <v>180</v>
+      </c>
+      <c r="E37" s="9" t="str">
+        <f>RIGHT(LEFT(C37,33),1)</f>
+        <v>8</v>
+      </c>
+      <c r="F37" s="10">
+        <f>10-E37</f>
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>10</v>
+      </c>
+      <c r="I37" t="str">
+        <f>"012"</f>
+        <v>012</v>
+      </c>
+      <c r="J37" s="10" t="str">
+        <f t="shared" ref="J37" si="41">_xlfn.TEXTJOIN("",FALSE,G37,":",H37,".",I37)</f>
+        <v>4:10.012</v>
+      </c>
+      <c r="K37" s="10">
+        <f t="shared" ref="K37" si="42">(G37*60)+(H37)+(I37/1000)</f>
+        <v>250.012</v>
+      </c>
+      <c r="L37" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38">
+        <v>180</v>
+      </c>
+      <c r="E38" s="9" t="str">
+        <f>RIGHT(LEFT(C38,33),1)</f>
+        <v>8</v>
+      </c>
+      <c r="F38" s="10">
+        <f>10-E38</f>
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>10</v>
+      </c>
+      <c r="I38" t="str">
+        <f>"012"</f>
+        <v>012</v>
+      </c>
+      <c r="J38" s="10" t="str">
+        <f t="shared" ref="J38" si="43">_xlfn.TEXTJOIN("",FALSE,G38,":",H38,".",I38)</f>
+        <v>4:10.012</v>
+      </c>
+      <c r="K38" s="10">
+        <f t="shared" ref="K38" si="44">(G38*60)+(H38)+(I38/1000)</f>
+        <v>250.012</v>
+      </c>
+      <c r="L38" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39">
+        <v>240</v>
+      </c>
+      <c r="E39" s="9" t="str">
+        <f>RIGHT(LEFT(C39,33),1)</f>
+        <v>5</v>
+      </c>
+      <c r="F39" s="10">
+        <f>10-E39</f>
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>10</v>
+      </c>
+      <c r="I39" t="str">
+        <f>"012"</f>
+        <v>012</v>
+      </c>
+      <c r="J39" s="10" t="str">
+        <f t="shared" ref="J39" si="45">_xlfn.TEXTJOIN("",FALSE,G39,":",H39,".",I39)</f>
+        <v>4:10.012</v>
+      </c>
+      <c r="K39" s="10">
+        <f t="shared" ref="K39" si="46">(G39*60)+(H39)+(I39/1000)</f>
+        <v>250.012</v>
+      </c>
+      <c r="L39" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40">
+        <v>270</v>
+      </c>
+      <c r="E40" s="9" t="str">
+        <f>RIGHT(LEFT(C40,33),1)</f>
+        <v>6</v>
+      </c>
+      <c r="F40" s="10">
+        <f>10-E40</f>
+        <v>4</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>10</v>
+      </c>
+      <c r="I40" t="str">
+        <f>"012"</f>
+        <v>012</v>
+      </c>
+      <c r="J40" s="10" t="str">
+        <f t="shared" ref="J40" si="47">_xlfn.TEXTJOIN("",FALSE,G40,":",H40,".",I40)</f>
+        <v>4:10.012</v>
+      </c>
+      <c r="K40" s="10">
+        <f t="shared" ref="K40" si="48">(G40*60)+(H40)+(I40/1000)</f>
+        <v>250.012</v>
+      </c>
+      <c r="L40" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B41" s="5">
+        <v>17</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="5">
+        <v>300</v>
+      </c>
+      <c r="E41" s="6" t="str">
+        <f>RIGHT(LEFT(C41,33),1)</f>
+        <v>9</v>
+      </c>
+      <c r="F41" s="5">
+        <f>10-E41</f>
+        <v>1</v>
+      </c>
+      <c r="G41" s="5">
+        <v>4</v>
+      </c>
+      <c r="H41" s="5" t="str">
+        <f>"03"</f>
+        <v>03</v>
+      </c>
+      <c r="I41" s="5">
+        <v>124</v>
+      </c>
+      <c r="J41" s="5" t="str">
+        <f t="shared" ref="J41" si="49">_xlfn.TEXTJOIN("",FALSE,G41,":",H41,".",I41)</f>
+        <v>4:03.124</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" ref="K41" si="50">(G41*60)+(H41)+(I41/1000)</f>
+        <v>243.124</v>
+      </c>
+      <c r="L41" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42">
+        <v>330</v>
+      </c>
+      <c r="E42" s="9" t="str">
+        <f>RIGHT(LEFT(C42,33),1)</f>
+        <v>9</v>
+      </c>
+      <c r="F42" s="10">
+        <f>10-E42</f>
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>4</v>
+      </c>
+      <c r="H42" t="str">
+        <f>"03"</f>
+        <v>03</v>
+      </c>
+      <c r="I42">
+        <v>124</v>
+      </c>
+      <c r="J42" s="10" t="str">
+        <f t="shared" ref="J42" si="51">_xlfn.TEXTJOIN("",FALSE,G42,":",H42,".",I42)</f>
+        <v>4:03.124</v>
+      </c>
+      <c r="K42" s="10">
+        <f t="shared" ref="K42" si="52">(G42*60)+(H42)+(I42/1000)</f>
+        <v>243.124</v>
+      </c>
+      <c r="L42" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B43" s="5">
+        <v>19</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="5">
+        <v>400</v>
+      </c>
+      <c r="E43" s="6" t="str">
+        <f>RIGHT(LEFT(C43,33),1)</f>
+        <v>7</v>
+      </c>
+      <c r="F43" s="5">
+        <f>10-E43</f>
+        <v>3</v>
+      </c>
+      <c r="G43" s="5">
+        <v>3</v>
+      </c>
+      <c r="H43" s="5">
+        <v>40</v>
+      </c>
+      <c r="I43" s="5">
+        <v>524</v>
+      </c>
+      <c r="J43" s="5" t="str">
+        <f t="shared" ref="J43" si="53">_xlfn.TEXTJOIN("",FALSE,G43,":",H43,".",I43)</f>
+        <v>3:40.524</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" ref="K43" si="54">(G43*60)+(H43)+(I43/1000)</f>
+        <v>220.524</v>
+      </c>
+      <c r="L43" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44">
+        <v>430</v>
+      </c>
+      <c r="E44" s="9" t="str">
+        <f>RIGHT(LEFT(C44,33),1)</f>
+        <v>7</v>
+      </c>
+      <c r="F44" s="10">
+        <f>10-E44</f>
+        <v>3</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
+      <c r="H44">
+        <v>40</v>
+      </c>
+      <c r="I44">
+        <v>524</v>
+      </c>
+      <c r="J44" s="10" t="str">
+        <f t="shared" ref="J44" si="55">_xlfn.TEXTJOIN("",FALSE,G44,":",H44,".",I44)</f>
+        <v>3:40.524</v>
+      </c>
+      <c r="K44" s="10">
+        <f t="shared" ref="K44" si="56">(G44*60)+(H44)+(I44/1000)</f>
+        <v>220.524</v>
+      </c>
+      <c r="L44" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45">
+        <v>500</v>
+      </c>
+      <c r="E45" s="9" t="str">
+        <f>RIGHT(LEFT(C45,33),1)</f>
+        <v>7</v>
+      </c>
+      <c r="F45" s="10">
+        <f>10-E45</f>
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45">
+        <v>40</v>
+      </c>
+      <c r="I45">
+        <v>524</v>
+      </c>
+      <c r="J45" s="10" t="str">
+        <f t="shared" ref="J45" si="57">_xlfn.TEXTJOIN("",FALSE,G45,":",H45,".",I45)</f>
+        <v>3:40.524</v>
+      </c>
+      <c r="K45" s="10">
+        <f t="shared" ref="K45" si="58">(G45*60)+(H45)+(I45/1000)</f>
+        <v>220.524</v>
+      </c>
+      <c r="L45" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>22</v>
+      </c>
+      <c r="C46" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46">
+        <v>500</v>
+      </c>
+      <c r="E46" s="9" t="str">
+        <f>RIGHT(LEFT(C46,33),1)</f>
+        <v>7</v>
+      </c>
+      <c r="F46" s="10">
+        <f>10-E46</f>
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>40</v>
+      </c>
+      <c r="I46">
+        <v>524</v>
+      </c>
+      <c r="J46" s="10" t="str">
+        <f t="shared" ref="J46" si="59">_xlfn.TEXTJOIN("",FALSE,G46,":",H46,".",I46)</f>
+        <v>3:40.524</v>
+      </c>
+      <c r="K46" s="10">
+        <f t="shared" ref="K46" si="60">(G46*60)+(H46)+(I46/1000)</f>
+        <v>220.524</v>
+      </c>
+      <c r="L46" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B47" s="5">
+        <v>23</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="5">
+        <v>530</v>
+      </c>
+      <c r="E47" s="6" t="str">
+        <f>RIGHT(LEFT(C47,33),1)</f>
+        <v>8</v>
+      </c>
+      <c r="F47" s="5">
+        <f>10-E47</f>
+        <v>2</v>
+      </c>
+      <c r="G47" s="5">
+        <v>3</v>
+      </c>
+      <c r="H47" s="5">
+        <v>35</v>
+      </c>
+      <c r="I47" s="5">
+        <v>991</v>
+      </c>
+      <c r="J47" s="5" t="str">
+        <f t="shared" ref="J47" si="61">_xlfn.TEXTJOIN("",FALSE,G47,":",H47,".",I47)</f>
+        <v>3:35.991</v>
+      </c>
+      <c r="K47" s="5">
+        <f t="shared" ref="K47" si="62">(G47*60)+(H47)+(I47/1000)</f>
+        <v>215.99100000000001</v>
+      </c>
+      <c r="L47" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48">
+        <v>600</v>
+      </c>
+      <c r="E48" s="9" t="str">
+        <f>RIGHT(LEFT(C48,33),1)</f>
+        <v>8</v>
+      </c>
+      <c r="F48" s="10">
+        <f>10-E48</f>
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <v>35</v>
+      </c>
+      <c r="I48">
+        <v>991</v>
+      </c>
+      <c r="J48" s="10" t="str">
+        <f t="shared" ref="J48" si="63">_xlfn.TEXTJOIN("",FALSE,G48,":",H48,".",I48)</f>
+        <v>3:35.991</v>
+      </c>
+      <c r="K48" s="10">
+        <f t="shared" ref="K48" si="64">(G48*60)+(H48)+(I48/1000)</f>
+        <v>215.99100000000001</v>
+      </c>
+      <c r="L48" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49">
+        <v>630</v>
+      </c>
+      <c r="E49" s="9" t="str">
+        <f>RIGHT(LEFT(C49,33),1)</f>
+        <v>7</v>
+      </c>
+      <c r="F49" s="10">
+        <f>10-E49</f>
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <v>35</v>
+      </c>
+      <c r="I49">
+        <v>991</v>
+      </c>
+      <c r="J49" s="10" t="str">
+        <f t="shared" ref="J49" si="65">_xlfn.TEXTJOIN("",FALSE,G49,":",H49,".",I49)</f>
+        <v>3:35.991</v>
+      </c>
+      <c r="K49" s="10">
+        <f t="shared" ref="K49" si="66">(G49*60)+(H49)+(I49/1000)</f>
+        <v>215.99100000000001</v>
+      </c>
+      <c r="L49" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>26</v>
+      </c>
+      <c r="C50" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50">
+        <v>700</v>
+      </c>
+      <c r="E50" s="9" t="str">
+        <f>RIGHT(LEFT(C50,33),1)</f>
+        <v>9</v>
+      </c>
+      <c r="F50" s="10">
+        <f>10-E50</f>
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="H50">
+        <v>35</v>
+      </c>
+      <c r="I50">
+        <v>991</v>
+      </c>
+      <c r="J50" s="10" t="str">
+        <f t="shared" ref="J50" si="67">_xlfn.TEXTJOIN("",FALSE,G50,":",H50,".",I50)</f>
+        <v>3:35.991</v>
+      </c>
+      <c r="K50" s="10">
+        <f t="shared" ref="K50" si="68">(G50*60)+(H50)+(I50/1000)</f>
+        <v>215.99100000000001</v>
+      </c>
+      <c r="L50" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>27</v>
+      </c>
+      <c r="C51" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51">
+        <v>730</v>
+      </c>
+      <c r="E51" s="9" t="str">
+        <f>RIGHT(LEFT(C51,33),1)</f>
+        <v>4</v>
+      </c>
+      <c r="F51" s="10">
+        <f>10-E51</f>
+        <v>6</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+      <c r="H51">
+        <v>35</v>
+      </c>
+      <c r="I51">
+        <v>991</v>
+      </c>
+      <c r="J51" s="10" t="str">
+        <f t="shared" ref="J51" si="69">_xlfn.TEXTJOIN("",FALSE,G51,":",H51,".",I51)</f>
+        <v>3:35.991</v>
+      </c>
+      <c r="K51" s="10">
+        <f t="shared" ref="K51" si="70">(G51*60)+(H51)+(I51/1000)</f>
+        <v>215.99100000000001</v>
+      </c>
+      <c r="L51" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54">
+        <f>3*60</f>
+        <v>180</v>
+      </c>
+      <c r="E54" t="s">
+        <v>51</v>
+      </c>
+      <c r="F54" t="s">
+        <v>51</v>
+      </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
+      <c r="H54">
+        <v>57</v>
+      </c>
+      <c r="I54">
+        <v>128</v>
+      </c>
+      <c r="J54" s="10" t="str">
+        <f t="shared" ref="J54" si="71">_xlfn.TEXTJOIN("",FALSE,G54,":",H54,".",I54)</f>
+        <v>3:57.128</v>
+      </c>
+      <c r="K54" s="10">
+        <f t="shared" ref="K54" si="72">(G54*60)+(H54)+(I54/1000)</f>
+        <v>237.12799999999999</v>
+      </c>
+      <c r="L54" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55">
+        <f>60*5</f>
+        <v>300</v>
+      </c>
+      <c r="E55" t="s">
+        <v>51</v>
+      </c>
+      <c r="F55" t="s">
+        <v>51</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>50</v>
+      </c>
+      <c r="I55">
+        <v>193</v>
+      </c>
+      <c r="J55" s="10" t="str">
+        <f t="shared" ref="J55" si="73">_xlfn.TEXTJOIN("",FALSE,G55,":",H55,".",I55)</f>
+        <v>3:50.193</v>
+      </c>
+      <c r="K55" s="10">
+        <f t="shared" ref="K55" si="74">(G55*60)+(H55)+(I55/1000)</f>
+        <v>230.19300000000001</v>
+      </c>
+      <c r="L55" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56">
+        <f>60*7</f>
+        <v>420</v>
+      </c>
+      <c r="E56" t="s">
+        <v>51</v>
+      </c>
+      <c r="F56" t="s">
+        <v>51</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>50</v>
+      </c>
+      <c r="I56">
+        <v>193</v>
+      </c>
+      <c r="J56" s="10" t="str">
+        <f t="shared" ref="J56" si="75">_xlfn.TEXTJOIN("",FALSE,G56,":",H56,".",I56)</f>
+        <v>3:50.193</v>
+      </c>
+      <c r="K56" s="10">
+        <f t="shared" ref="K56" si="76">(G56*60)+(H56)+(I56/1000)</f>
+        <v>230.19300000000001</v>
+      </c>
+      <c r="L56" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57">
+        <f>60*10</f>
+        <v>600</v>
+      </c>
+      <c r="E57" t="s">
+        <v>51</v>
+      </c>
+      <c r="F57" t="s">
+        <v>51</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
+      <c r="H57">
+        <v>50</v>
+      </c>
+      <c r="I57">
+        <v>193</v>
+      </c>
+      <c r="J57" s="10" t="str">
+        <f t="shared" ref="J57" si="77">_xlfn.TEXTJOIN("",FALSE,G57,":",H57,".",I57)</f>
+        <v>3:50.193</v>
+      </c>
+      <c r="K57" s="10">
+        <f t="shared" ref="K57" si="78">(G57*60)+(H57)+(I57/1000)</f>
+        <v>230.19300000000001</v>
+      </c>
+      <c r="L57" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59">
+        <f>3*60</f>
+        <v>180</v>
+      </c>
+      <c r="E59" t="s">
+        <v>51</v>
+      </c>
+      <c r="F59" t="s">
+        <v>51</v>
+      </c>
+      <c r="G59">
+        <v>3</v>
+      </c>
+      <c r="H59">
+        <v>50</v>
+      </c>
+      <c r="I59">
+        <v>138</v>
+      </c>
+      <c r="J59" s="10" t="str">
+        <f t="shared" ref="J59:J62" si="79">_xlfn.TEXTJOIN("",FALSE,G59,":",H59,".",I59)</f>
+        <v>3:50.138</v>
+      </c>
+      <c r="K59" s="10">
+        <f t="shared" ref="K59:K62" si="80">(G59*60)+(H59)+(I59/1000)</f>
+        <v>230.13800000000001</v>
+      </c>
+      <c r="L59" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60">
+        <f>6*60</f>
+        <v>360</v>
+      </c>
+      <c r="E60" t="s">
+        <v>51</v>
+      </c>
+      <c r="F60" t="s">
+        <v>51</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+      <c r="H60">
+        <v>47</v>
+      </c>
+      <c r="I60">
+        <v>922</v>
+      </c>
+      <c r="J60" s="10" t="str">
+        <f t="shared" si="79"/>
+        <v>3:47.922</v>
+      </c>
+      <c r="K60" s="10">
+        <f t="shared" si="80"/>
+        <v>227.922</v>
+      </c>
+      <c r="L60" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61">
+        <f>8*60</f>
+        <v>480</v>
+      </c>
+      <c r="E61" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" t="s">
+        <v>51</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <v>41</v>
+      </c>
+      <c r="I61">
+        <v>660</v>
+      </c>
+      <c r="J61" s="10" t="str">
+        <f t="shared" si="79"/>
+        <v>3:41.660</v>
+      </c>
+      <c r="K61" s="10">
+        <f t="shared" si="80"/>
+        <v>221.66</v>
+      </c>
+      <c r="L61" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62">
+        <f>9*60</f>
+        <v>540</v>
+      </c>
+      <c r="E62" t="s">
+        <v>51</v>
+      </c>
+      <c r="F62" t="s">
+        <v>51</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+      <c r="H62">
+        <v>41</v>
+      </c>
+      <c r="I62">
+        <v>456</v>
+      </c>
+      <c r="J62" s="10" t="str">
+        <f t="shared" si="79"/>
+        <v>3:41.456</v>
+      </c>
+      <c r="K62" s="10">
+        <f t="shared" si="80"/>
+        <v>221.45599999999999</v>
+      </c>
+      <c r="L62" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63">
+        <v>600</v>
+      </c>
+      <c r="E63" t="s">
+        <v>51</v>
+      </c>
+      <c r="F63" t="s">
+        <v>51</v>
+      </c>
+      <c r="G63">
+        <v>3</v>
+      </c>
+      <c r="H63">
+        <v>41</v>
+      </c>
+      <c r="I63">
+        <v>456</v>
+      </c>
+      <c r="J63" s="10" t="str">
+        <f t="shared" ref="J63" si="81">_xlfn.TEXTJOIN("",FALSE,G63,":",H63,".",I63)</f>
+        <v>3:41.456</v>
+      </c>
+      <c r="K63" s="10">
+        <f t="shared" ref="K63" si="82">(G63*60)+(H63)+(I63/1000)</f>
+        <v>221.45599999999999</v>
+      </c>
+      <c r="L63" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B64" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65">
+        <f>3*60</f>
+        <v>180</v>
+      </c>
+      <c r="E65" t="s">
+        <v>51</v>
+      </c>
+      <c r="F65" t="s">
+        <v>51</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+      <c r="H65">
+        <v>57</v>
+      </c>
+      <c r="I65">
+        <v>594</v>
+      </c>
+      <c r="J65" s="10" t="str">
+        <f t="shared" ref="J65" si="83">_xlfn.TEXTJOIN("",FALSE,G65,":",H65,".",I65)</f>
+        <v>3:57.594</v>
+      </c>
+      <c r="K65" s="10">
+        <f t="shared" ref="K65" si="84">(G65*60)+(H65)+(I65/1000)</f>
+        <v>237.59399999999999</v>
+      </c>
+      <c r="L65" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>71</v>
+      </c>
+      <c r="D66">
+        <f>6*60</f>
+        <v>360</v>
+      </c>
+      <c r="E66" t="s">
+        <v>51</v>
+      </c>
+      <c r="F66" t="s">
+        <v>51</v>
+      </c>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="20">
+    <mergeCell ref="B58:L58"/>
+    <mergeCell ref="B64:L64"/>
     <mergeCell ref="A17:A23"/>
     <mergeCell ref="B4:L4"/>
     <mergeCell ref="B24:L24"/>
     <mergeCell ref="A25:A31"/>
+    <mergeCell ref="B53:L53"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="J2:K3"/>

</xml_diff>